<commit_message>
Add About page note for FoVBPD
</commit_message>
<xml_diff>
--- a/InputData/trans/FoVBPD/Fraction of Vehicle Batteries Produced Domestically.xlsx
+++ b/InputData/trans/FoVBPD/Fraction of Vehicle Batteries Produced Domestically.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\FoVBPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9489379-3480-48D4-9782-54A82A12852F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AECF23-A61B-44F8-B5D9-89EF6743C0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{DC12087C-9A27-4A43-B4A9-6B3F1E517F08}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DC12087C-9A27-4A43-B4A9-6B3F1E517F08}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Sources:</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>Table 1</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>This variable affects what portion of newly sold vehicles qualify for Vehicle Battery Production subsidy,</t>
+  </si>
+  <si>
+    <t>if relevant. We assume that the U.S. has enough battery manufacturing capacity to supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% of vehicle battery demand domestically. All U.S. state models should use the U.S. vaues, since the </t>
+  </si>
+  <si>
+    <t>battery manufacturing production tax credit applies to all U.S. manufactured batteries.</t>
   </si>
 </sst>
 </file>
@@ -424,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF982137-6F01-4109-8226-D4C6F3731BA9}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,6 +485,31 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>